<commit_message>
Added some functions for directory manipulation to the useful functions namespace. Some minor edits to the testing namespace.
</commit_message>
<xml_diff>
--- a/Spectrum/Spectrum/Plots.xlsx
+++ b/Spectrum/Spectrum/Plots.xlsx
@@ -15,8 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.0" hidden="1">Sheet1!$A$2:$A$1101</definedName>
-    <definedName name="_xlchart.1" hidden="1">Sheet1!$B$2:$B$1101</definedName>
     <definedName name="Spec_Data" localSheetId="0">Sheet1!$B$2:$B$1101</definedName>
     <definedName name="Spec_Data_Abs_FFT_data" localSheetId="0">Sheet1!$D$2:$D$1025</definedName>
     <definedName name="Spec_Data_Frq_data" localSheetId="0">Sheet1!$C$2:$C$1025</definedName>
@@ -14732,15 +14730,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15043,8 +15041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E2:E1025"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>